<commit_message>
Comentando Script e Atualizando Backlogs
</commit_message>
<xml_diff>
--- a/Docs/ProductBacklog-v2.xlsx
+++ b/Docs/ProductBacklog-v2.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\projeto-pi\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\coold\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="237"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="237" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="SprintBacklog" sheetId="2" r:id="rId2"/>
+    <sheet name="SprintBacklog2" sheetId="2" r:id="rId2"/>
+    <sheet name="SprintBacklog3" sheetId="3" r:id="rId3"/>
+    <sheet name="SprintBacklog4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="30">
   <si>
     <t>Escopo</t>
   </si>
@@ -99,9 +101,6 @@
     <t>Fazer a modelagem conceitual dos dados que irão compor as tabelas</t>
   </si>
   <si>
-    <t>Sprint Grupo 1 (Sprint 2)- 16/09 - 23/09</t>
-  </si>
-  <si>
     <t>O site deverá ter uma tela de cadastro do usuário (Nome, Sobrenome, Email, Telefone, CNPJ, senha)</t>
   </si>
   <si>
@@ -109,6 +108,15 @@
   </si>
   <si>
     <t>Product Backlog</t>
+  </si>
+  <si>
+    <t>Sprint Grupo 1 (Sprint 2)- 16/09 - 30/09</t>
+  </si>
+  <si>
+    <t>Sprint Grupo 1 (Sprint 3)- 30/09 - 14/10</t>
+  </si>
+  <si>
+    <t>Sprint Grupo 1 (Sprint 3)- 14/10 - 21/10</t>
   </si>
 </sst>
 </file>
@@ -209,7 +217,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -293,11 +301,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -385,6 +402,13 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,7 +691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -955,7 +979,7 @@
     <row r="21" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>15</v>
@@ -976,6 +1000,312 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="137" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="9">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="25">
+        <v>4</v>
+      </c>
+      <c r="D5" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="25">
+        <v>5</v>
+      </c>
+      <c r="D6" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <v>6</v>
+      </c>
+      <c r="B7" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="28">
+        <v>6</v>
+      </c>
+      <c r="D7" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="25">
+        <v>7</v>
+      </c>
+      <c r="D8" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <v>8</v>
+      </c>
+      <c r="B9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="28">
+        <v>8</v>
+      </c>
+      <c r="D9" s="26">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <v>11</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="25">
+        <v>3</v>
+      </c>
+      <c r="D12" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>13</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="35">
+        <v>2</v>
+      </c>
+      <c r="D14" s="36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <v>14</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="25">
+        <v>3</v>
+      </c>
+      <c r="D15" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="27">
+        <v>15</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="25">
+        <v>4</v>
+      </c>
+      <c r="D16" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>16</v>
+      </c>
+      <c r="B17" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="25">
+        <v>5</v>
+      </c>
+      <c r="D17" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>17</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="31">
+        <v>6</v>
+      </c>
+      <c r="D18" s="32">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
+        <v>18</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="25">
+        <v>7</v>
+      </c>
+      <c r="D19" s="33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="20">
+        <f>SUM(D2,D3,D4,D10,D11,D13,D14)</f>
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -1004,73 +1334,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="28">
+        <v>1</v>
+      </c>
+      <c r="D2" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="9">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="C3" s="28">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="9">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
+      <c r="D3" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="9">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="C4" s="28">
+        <v>3</v>
+      </c>
+      <c r="D4" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="9">
         <v>4</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="11">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="23">
-        <v>5</v>
-      </c>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="7">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="25">
-        <v>5</v>
-      </c>
-      <c r="D6" s="26">
+      <c r="C6" s="9">
+        <v>5</v>
+      </c>
+      <c r="D6" s="11">
         <v>3</v>
       </c>
     </row>
@@ -1117,30 +1447,30 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="23">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="25">
         <v>1</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="26">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
+      <c r="A11" s="23">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="25">
         <v>2</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="26">
         <v>3</v>
       </c>
     </row>
@@ -1148,7 +1478,7 @@
       <c r="A12" s="23">
         <v>11</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="24" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="25">
@@ -1159,7 +1489,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="A13" s="34">
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
@@ -1168,7 +1498,7 @@
       <c r="C13" s="9">
         <v>1</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="11">
         <v>3</v>
       </c>
     </row>
@@ -1190,7 +1520,7 @@
       <c r="A15" s="23">
         <v>14</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="24" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="25">
@@ -1201,16 +1531,16 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="27">
+      <c r="A16" s="34">
         <v>15</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="25">
+      <c r="C16" s="35">
         <v>4</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="36">
         <v>8</v>
       </c>
     </row>
@@ -1265,18 +1595,322 @@
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C21" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D21" s="20">
-        <f>SUM(D2,D3,D4,D10,D11,D13,D14)</f>
-        <v>33</v>
+        <f>SUM(D14,D16,D5:D6,D13)</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="137" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="28">
+        <v>1</v>
+      </c>
+      <c r="D2" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="28">
+        <v>2</v>
+      </c>
+      <c r="D3" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="27">
+        <v>3</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="28">
+        <v>3</v>
+      </c>
+      <c r="D4" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <v>4</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="28">
+        <v>4</v>
+      </c>
+      <c r="D5" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <v>5</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="28">
+        <v>5</v>
+      </c>
+      <c r="D6" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="9">
+        <v>6</v>
+      </c>
+      <c r="D7" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="9">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="9">
+        <v>8</v>
+      </c>
+      <c r="D9" s="11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <v>9</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="25">
+        <v>1</v>
+      </c>
+      <c r="D10" s="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>10</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="25">
+        <v>2</v>
+      </c>
+      <c r="D11" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3</v>
+      </c>
+      <c r="D12" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="39">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="38">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="39">
+        <v>2</v>
+      </c>
+      <c r="D14" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="38">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="39">
+        <v>3</v>
+      </c>
+      <c r="D15" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="39">
+        <v>4</v>
+      </c>
+      <c r="D16" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="23">
+        <v>16</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="25">
+        <v>5</v>
+      </c>
+      <c r="D17" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="23">
+        <v>17</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="25">
+        <v>6</v>
+      </c>
+      <c r="D18" s="26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="23">
+        <v>18</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="25">
+        <v>7</v>
+      </c>
+      <c r="D19" s="26">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="37"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="20">
+        <f>SUM(D12:D16,D7:D9)</f>
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>